<commit_message>
Añadiendo Serie2_PEA_MX y diagnosticando con métodos estáticos y de HOLT winters. FALTA ANÁLISIS DE RESULTADOS
</commit_message>
<xml_diff>
--- a/PEA_MEX_full.xlsx
+++ b/PEA_MEX_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9e6e0322c927b48/Documentos/MIS_UNAM/Segundo_semestre/Series_UNAM_HPi3/Series_UNAM_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{E99F2E2B-D287-4391-8EC6-4A0A1E93C84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4528F2-CFE7-4875-BFC1-0AB0FA195F9C}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{E99F2E2B-D287-4391-8EC6-4A0A1E93C84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BAD786F-7B9E-4654-B37D-FB00AC8F22CC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9C482A4-B857-436F-9DC5-C4D7D20035FB}"/>
   </bookViews>
@@ -96,6 +96,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,9 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56C9B97-9B1C-404C-8FDA-8FD68F7658A2}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -945,28 +947,52 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
+      <c r="A68" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B68">
+        <v>58307446</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
+      <c r="A69" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B69">
+        <v>58761793</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
+      <c r="A70" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B70">
+        <v>58085314</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="2"/>
+      <c r="A71" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B71">
+        <v>59338419</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
+      <c r="A72" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B72">
+        <v>59480471</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2"/>
+      <c r="A73" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B73">
+        <v>60145456</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>